<commit_message>
Update test suite for InterestRateCalculator
</commit_message>
<xml_diff>
--- a/05-Test/Testsuites/InterestRateCalculator.xlsx
+++ b/05-Test/Testsuites/InterestRateCalculator.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AppData\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AppData\GitHub\DMU14EksamensProjekt2sem\05-Test\Testsuites\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13728"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13728" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ækvivalensklasser" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="30">
   <si>
     <t>Løbetid</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Klasse#</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Exception: Null pointer:</t>
+  </si>
+  <si>
+    <t>Kreditværdighed kan ikke være null</t>
   </si>
 </sst>
 </file>
@@ -539,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,7 +792,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="24" t="s">
         <v>17</v>
       </c>
@@ -798,11 +807,9 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>6</v>
-      </c>
+      <c r="B19" s="28"/>
       <c r="C19" s="24" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D19" s="25">
         <v>0.5</v>
@@ -816,7 +823,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C20" s="24" t="s">
         <v>8</v>
@@ -832,78 +839,95 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="24">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="30">
+      <c r="C22" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="30">
         <v>0.5</v>
       </c>
-      <c r="E21" s="29">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="29">
+        <v>37</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="28">
-        <v>0.01</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="28">
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="28">
         <v>0.49990000000000001</v>
       </c>
-      <c r="E24" s="27">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="25">
+      <c r="E25" s="27">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="25">
         <v>0.9998999999999999</v>
       </c>
-      <c r="E25" s="24">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="3">
+      <c r="E26" s="24">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3">
         <v>0.5</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E27" s="2">
         <v>1</v>
       </c>
     </row>
@@ -916,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,6 +2058,20 @@
       <c r="E46" s="4">
         <v>0.05</v>
       </c>
+      <c r="F46" s="10">
+        <v>24</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J46" s="8"/>
+      <c r="K46" s="7"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
@@ -2045,6 +2083,18 @@
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J47" s="8"/>
+      <c r="K47" s="7"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
@@ -2056,8 +2106,18 @@
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" s="10"/>
+      <c r="G48" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H48" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="I48" s="9"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="s">
         <v>0</v>
@@ -2067,6 +2127,16 @@
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H49" s="10">
+        <v>37</v>
+      </c>
+      <c r="I49" s="9"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>